<commit_message>
actual final session logs
</commit_message>
<xml_diff>
--- a/mVR_session_log.xlsx
+++ b/mVR_session_log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="22">
   <si>
     <t>Animal #</t>
   </si>
@@ -155,8 +155,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -242,7 +246,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -281,6 +285,8 @@
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -319,6 +325,8 @@
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -648,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E140"/>
+  <dimension ref="B2:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F141" sqref="F141"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1580,26 +1588,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="2:5">
-      <c r="B99">
-        <v>152</v>
-      </c>
-      <c r="C99">
-        <v>104</v>
-      </c>
-      <c r="D99" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="100" spans="2:5">
-      <c r="B100">
-        <v>152</v>
-      </c>
-      <c r="C100">
-        <v>108</v>
-      </c>
-      <c r="D100" t="s">
-        <v>6</v>
+    <row r="98" spans="2:5">
+      <c r="B98">
+        <v>146</v>
+      </c>
+      <c r="C98">
+        <v>135</v>
+      </c>
+      <c r="D98" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="101" spans="2:5">
@@ -1607,10 +1604,10 @@
         <v>152</v>
       </c>
       <c r="C101">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D101" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="102" spans="2:5">
@@ -1618,10 +1615,10 @@
         <v>152</v>
       </c>
       <c r="C102">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D102" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103" spans="2:5">
@@ -1629,13 +1626,10 @@
         <v>152</v>
       </c>
       <c r="C103">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D103" t="s">
-        <v>9</v>
-      </c>
-      <c r="E103" s="4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="104" spans="2:5">
@@ -1643,13 +1637,10 @@
         <v>152</v>
       </c>
       <c r="C104">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D104" t="s">
-        <v>9</v>
-      </c>
-      <c r="E104" s="4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105" spans="2:5">
@@ -1657,7 +1648,7 @@
         <v>152</v>
       </c>
       <c r="C105">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D105" t="s">
         <v>9</v>
@@ -1671,7 +1662,7 @@
         <v>152</v>
       </c>
       <c r="C106">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D106" t="s">
         <v>9</v>
@@ -1680,26 +1671,32 @@
         <v>17</v>
       </c>
     </row>
+    <row r="107" spans="2:5">
+      <c r="B107">
+        <v>152</v>
+      </c>
+      <c r="C107">
+        <v>127</v>
+      </c>
+      <c r="D107" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="108" spans="2:5">
       <c r="B108">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C108">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="D108" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="109" spans="2:5">
-      <c r="B109">
-        <v>153</v>
-      </c>
-      <c r="C109">
-        <v>148</v>
-      </c>
-      <c r="D109" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="110" spans="2:5">
@@ -1707,10 +1704,10 @@
         <v>153</v>
       </c>
       <c r="C110">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D110" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="111" spans="2:5">
@@ -1718,10 +1715,10 @@
         <v>153</v>
       </c>
       <c r="C111">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D111" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="112" spans="2:5">
@@ -1729,7 +1726,7 @@
         <v>153</v>
       </c>
       <c r="C112">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D112" t="s">
         <v>9</v>
@@ -1740,10 +1737,10 @@
         <v>153</v>
       </c>
       <c r="C113">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D113" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="114" spans="2:5">
@@ -1751,10 +1748,10 @@
         <v>153</v>
       </c>
       <c r="C114">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D114" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="115" spans="2:5">
@@ -1762,7 +1759,7 @@
         <v>153</v>
       </c>
       <c r="C115">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D115" t="s">
         <v>16</v>
@@ -1773,35 +1770,35 @@
         <v>153</v>
       </c>
       <c r="C116">
+        <v>167</v>
+      </c>
+      <c r="D116" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5">
+      <c r="B117">
+        <v>153</v>
+      </c>
+      <c r="C117">
+        <v>170</v>
+      </c>
+      <c r="D117" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5">
+      <c r="B118">
+        <v>153</v>
+      </c>
+      <c r="C118">
         <v>171</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D118" t="s">
         <v>18</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E118" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="119" spans="2:5">
-      <c r="B119">
-        <v>154</v>
-      </c>
-      <c r="C119">
-        <v>144</v>
-      </c>
-      <c r="D119" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="120" spans="2:5">
-      <c r="B120">
-        <v>154</v>
-      </c>
-      <c r="C120">
-        <v>149</v>
-      </c>
-      <c r="D120" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="121" spans="2:5">
@@ -1809,10 +1806,10 @@
         <v>154</v>
       </c>
       <c r="C121">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D121" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="122" spans="2:5">
@@ -1820,10 +1817,10 @@
         <v>154</v>
       </c>
       <c r="C122">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D122" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="123" spans="2:5">
@@ -1831,7 +1828,7 @@
         <v>154</v>
       </c>
       <c r="C123">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D123" t="s">
         <v>9</v>
@@ -1842,10 +1839,10 @@
         <v>154</v>
       </c>
       <c r="C124">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D124" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="125" spans="2:5">
@@ -1853,10 +1850,10 @@
         <v>154</v>
       </c>
       <c r="C125">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D125" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="126" spans="2:5">
@@ -1864,51 +1861,48 @@
         <v>154</v>
       </c>
       <c r="C126">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D126" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="127" spans="2:5">
+      <c r="B127">
+        <v>154</v>
+      </c>
+      <c r="C127">
+        <v>166</v>
+      </c>
+      <c r="D127" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="128" spans="2:5">
       <c r="B128">
+        <v>154</v>
+      </c>
+      <c r="C128">
+        <v>168</v>
+      </c>
+      <c r="D128" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5">
+      <c r="B130">
         <v>155</v>
       </c>
-      <c r="C128">
+      <c r="C130">
         <v>145</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D130" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="2:5">
-      <c r="D129" t="s">
+    <row r="131" spans="2:5">
+      <c r="D131" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="133" spans="2:5">
-      <c r="B133">
-        <v>156</v>
-      </c>
-      <c r="C133">
-        <v>146</v>
-      </c>
-      <c r="D133" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="134" spans="2:5">
-      <c r="B134">
-        <v>156</v>
-      </c>
-      <c r="C134">
-        <v>151</v>
-      </c>
-      <c r="D134" t="s">
-        <v>7</v>
-      </c>
-      <c r="E134" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="135" spans="2:5">
@@ -1916,57 +1910,60 @@
         <v>156</v>
       </c>
       <c r="C135">
+        <v>146</v>
+      </c>
+      <c r="D135" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5">
+      <c r="B136">
+        <v>156</v>
+      </c>
+      <c r="C136">
+        <v>151</v>
+      </c>
+      <c r="D136" t="s">
+        <v>7</v>
+      </c>
+      <c r="E136" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5">
+      <c r="B137">
+        <v>156</v>
+      </c>
+      <c r="C137">
         <v>155</v>
       </c>
-      <c r="D135" t="s">
-        <v>9</v>
-      </c>
-      <c r="E135" t="s">
+      <c r="D137" t="s">
+        <v>9</v>
+      </c>
+      <c r="E137" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="136" spans="2:5">
-      <c r="B136" s="3">
+    <row r="138" spans="2:5">
+      <c r="B138" s="3">
         <v>156</v>
       </c>
-      <c r="C136">
+      <c r="C138">
         <v>157</v>
       </c>
-      <c r="D136" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="137" spans="2:5">
-      <c r="B137" s="3">
+      <c r="D138" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5">
+      <c r="B139" s="3">
         <v>156</v>
       </c>
-      <c r="C137">
+      <c r="C139">
         <v>160</v>
       </c>
-      <c r="D137" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="138" spans="2:5">
-      <c r="B138">
-        <v>156</v>
-      </c>
-      <c r="C138">
-        <v>162</v>
-      </c>
-      <c r="D138" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="139" spans="2:5">
-      <c r="B139">
-        <v>156</v>
-      </c>
-      <c r="C139">
-        <v>165</v>
-      </c>
       <c r="D139" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="140" spans="2:5">
@@ -1974,9 +1971,31 @@
         <v>156</v>
       </c>
       <c r="C140">
+        <v>162</v>
+      </c>
+      <c r="D140" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5">
+      <c r="B141">
+        <v>156</v>
+      </c>
+      <c r="C141">
+        <v>165</v>
+      </c>
+      <c r="D141" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5">
+      <c r="B142">
+        <v>156</v>
+      </c>
+      <c r="C142">
         <v>169</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D142" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>